<commit_message>
Manual match tables auto height adjust
</commit_message>
<xml_diff>
--- a/Resources/New Geo to Steel_MATCHED.xlsx
+++ b/Resources/New Geo to Steel_MATCHED.xlsx
@@ -76,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -148,6 +148,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -2821,220 +2830,172 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="9" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B70" s="10" t="inlineStr"/>
-      <c r="C70" s="11" t="inlineStr">
+      <c r="A70" s="1" t="inlineStr"/>
+      <c r="B70" s="2" t="inlineStr"/>
+      <c r="C70" s="6" t="inlineStr">
         <is>
           <t>24/Dec/2025</t>
         </is>
       </c>
-      <c r="D70" s="9" t="inlineStr">
+      <c r="D70" s="1" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E70" s="12" t="inlineStr">
+      <c r="E70" s="7" t="inlineStr">
         <is>
           <t>Brac Bank PLC-CD-A/C-2028701210002</t>
         </is>
       </c>
-      <c r="F70" s="9" t="inlineStr"/>
-      <c r="G70" s="9" t="inlineStr"/>
-      <c r="H70" s="13" t="inlineStr">
+      <c r="F70" s="1" t="inlineStr"/>
+      <c r="G70" s="1" t="inlineStr"/>
+      <c r="H70" s="25" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I70" s="9" t="inlineStr">
+      <c r="I70" s="1" t="inlineStr">
         <is>
           <t>67</t>
         </is>
       </c>
-      <c r="J70" s="9" t="inlineStr"/>
-      <c r="K70" s="14" t="inlineStr">
+      <c r="J70" s="1" t="inlineStr"/>
+      <c r="K70" s="8" t="inlineStr">
         <is>
           <t>45000000</t>
         </is>
       </c>
-      <c r="L70" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="L70" s="1" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" s="9" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B71" s="10" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 45000000.00
-Borrower Amount: 45000000.00</t>
-        </is>
-      </c>
-      <c r="C71" s="9" t="inlineStr"/>
-      <c r="D71" s="9" t="inlineStr"/>
-      <c r="E71" s="15" t="inlineStr">
+      <c r="A71" s="1" t="inlineStr"/>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>Unmatched Record
+Reasons:
+1. Borrower's narration does not contain lender's short code</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr"/>
+      <c r="D71" s="1" t="inlineStr"/>
+      <c r="E71" s="26" t="inlineStr">
         <is>
           <t>Interunit Funs Transfer as Interunit Loan A/C-Steel Unit, MTB# 1105</t>
         </is>
       </c>
-      <c r="F71" s="9" t="inlineStr"/>
-      <c r="G71" s="9" t="inlineStr"/>
-      <c r="H71" s="9" t="inlineStr"/>
-      <c r="I71" s="9" t="inlineStr"/>
-      <c r="J71" s="9" t="inlineStr"/>
-      <c r="K71" s="9" t="inlineStr"/>
-      <c r="L71" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F71" s="1" t="inlineStr"/>
+      <c r="G71" s="1" t="inlineStr"/>
+      <c r="H71" s="1" t="inlineStr"/>
+      <c r="I71" s="1" t="inlineStr"/>
+      <c r="J71" s="1" t="inlineStr"/>
+      <c r="K71" s="1" t="inlineStr"/>
+      <c r="L71" s="1" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" s="9" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B72" s="10" t="inlineStr"/>
-      <c r="C72" s="9" t="inlineStr"/>
-      <c r="D72" s="9" t="inlineStr">
+      <c r="A72" s="1" t="inlineStr"/>
+      <c r="B72" s="2" t="inlineStr"/>
+      <c r="C72" s="1" t="inlineStr"/>
+      <c r="D72" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E72" s="16" t="inlineStr">
+      <c r="E72" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F72" s="9" t="inlineStr"/>
-      <c r="G72" s="9" t="inlineStr"/>
-      <c r="H72" s="9" t="inlineStr"/>
-      <c r="I72" s="9" t="inlineStr"/>
-      <c r="J72" s="9" t="inlineStr"/>
-      <c r="K72" s="9" t="inlineStr"/>
-      <c r="L72" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F72" s="1" t="inlineStr"/>
+      <c r="G72" s="1" t="inlineStr"/>
+      <c r="H72" s="1" t="inlineStr"/>
+      <c r="I72" s="1" t="inlineStr"/>
+      <c r="J72" s="1" t="inlineStr"/>
+      <c r="K72" s="1" t="inlineStr"/>
+      <c r="L72" s="1" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" s="17" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B73" s="18" t="inlineStr"/>
-      <c r="C73" s="19" t="inlineStr">
+      <c r="A73" s="1" t="inlineStr"/>
+      <c r="B73" s="2" t="inlineStr"/>
+      <c r="C73" s="6" t="inlineStr">
         <is>
           <t>28/Dec/2025</t>
         </is>
       </c>
-      <c r="D73" s="17" t="inlineStr">
+      <c r="D73" s="1" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E73" s="20" t="inlineStr">
+      <c r="E73" s="7" t="inlineStr">
         <is>
           <t>Brac Bank PLC-CD-A/C-2028701210002</t>
         </is>
       </c>
-      <c r="F73" s="17" t="inlineStr"/>
-      <c r="G73" s="17" t="inlineStr"/>
-      <c r="H73" s="21" t="inlineStr">
+      <c r="F73" s="1" t="inlineStr"/>
+      <c r="G73" s="1" t="inlineStr"/>
+      <c r="H73" s="25" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I73" s="17" t="inlineStr">
+      <c r="I73" s="1" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="J73" s="17" t="inlineStr"/>
-      <c r="K73" s="22" t="inlineStr">
+      <c r="J73" s="1" t="inlineStr"/>
+      <c r="K73" s="8" t="inlineStr">
         <is>
           <t>100000</t>
         </is>
       </c>
-      <c r="L73" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="L73" s="1" t="inlineStr"/>
     </row>
     <row r="74">
-      <c r="A74" s="17" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B74" s="18" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 100000.00
-Borrower Amount: 100000.00</t>
-        </is>
-      </c>
-      <c r="C74" s="17" t="inlineStr"/>
-      <c r="D74" s="17" t="inlineStr"/>
-      <c r="E74" s="23" t="inlineStr">
+      <c r="A74" s="1" t="inlineStr"/>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>Unmatched Record
+Reasons:
+1. Borrower's narration does not contain lender's short code</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="inlineStr"/>
+      <c r="D74" s="1" t="inlineStr"/>
+      <c r="E74" s="26" t="inlineStr">
         <is>
           <t>Interunit Funs Transfer as Interunit Loan A/C-Steel Unit, MTB# 1105</t>
         </is>
       </c>
-      <c r="F74" s="17" t="inlineStr"/>
-      <c r="G74" s="17" t="inlineStr"/>
-      <c r="H74" s="17" t="inlineStr"/>
-      <c r="I74" s="17" t="inlineStr"/>
-      <c r="J74" s="17" t="inlineStr"/>
-      <c r="K74" s="17" t="inlineStr"/>
-      <c r="L74" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F74" s="1" t="inlineStr"/>
+      <c r="G74" s="1" t="inlineStr"/>
+      <c r="H74" s="1" t="inlineStr"/>
+      <c r="I74" s="1" t="inlineStr"/>
+      <c r="J74" s="1" t="inlineStr"/>
+      <c r="K74" s="1" t="inlineStr"/>
+      <c r="L74" s="1" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" s="17" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B75" s="18" t="inlineStr"/>
-      <c r="C75" s="17" t="inlineStr"/>
-      <c r="D75" s="17" t="inlineStr">
+      <c r="A75" s="1" t="inlineStr"/>
+      <c r="B75" s="2" t="inlineStr"/>
+      <c r="C75" s="1" t="inlineStr"/>
+      <c r="D75" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E75" s="24" t="inlineStr">
+      <c r="E75" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F75" s="17" t="inlineStr"/>
-      <c r="G75" s="17" t="inlineStr"/>
-      <c r="H75" s="17" t="inlineStr"/>
-      <c r="I75" s="17" t="inlineStr"/>
-      <c r="J75" s="17" t="inlineStr"/>
-      <c r="K75" s="17" t="inlineStr"/>
-      <c r="L75" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F75" s="1" t="inlineStr"/>
+      <c r="G75" s="1" t="inlineStr"/>
+      <c r="H75" s="1" t="inlineStr"/>
+      <c r="I75" s="1" t="inlineStr"/>
+      <c r="J75" s="1" t="inlineStr"/>
+      <c r="K75" s="1" t="inlineStr"/>
+      <c r="L75" s="1" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="9" t="inlineStr">
@@ -3375,7 +3336,7 @@
       <c r="H85" s="1" t="inlineStr"/>
       <c r="I85" s="1" t="inlineStr"/>
       <c r="J85" s="1" t="inlineStr"/>
-      <c r="K85" s="25" t="inlineStr">
+      <c r="K85" s="28" t="inlineStr">
         <is>
           <t>413172115.16</t>
         </is>
@@ -3423,7 +3384,7 @@
       <c r="H87" s="1" t="inlineStr"/>
       <c r="I87" s="1" t="inlineStr"/>
       <c r="J87" s="1" t="inlineStr"/>
-      <c r="K87" s="25" t="inlineStr">
+      <c r="K87" s="28" t="inlineStr">
         <is>
           <t>413172115.16</t>
         </is>

</xml_diff>

<commit_message>
Process log updated to consistent formatting
</commit_message>
<xml_diff>
--- a/Resources/New Geo to Steel_MATCHED.xlsx
+++ b/Resources/New Geo to Steel_MATCHED.xlsx
@@ -76,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -148,15 +148,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1950,7 +1941,7 @@
     <row r="45">
       <c r="A45" s="17" t="inlineStr">
         <is>
-          <t>M001</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="B45" s="18" t="inlineStr"/>
@@ -1996,7 +1987,7 @@
     <row r="46">
       <c r="A46" s="17" t="inlineStr">
         <is>
-          <t>M001</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="B46" s="18" t="inlineStr">
@@ -2028,7 +2019,7 @@
     <row r="47">
       <c r="A47" s="17" t="inlineStr">
         <is>
-          <t>M001</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="B47" s="18" t="inlineStr"/>
@@ -2824,172 +2815,220 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr"/>
-      <c r="B70" s="2" t="inlineStr"/>
-      <c r="C70" s="6" t="inlineStr">
+      <c r="A70" s="9" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B70" s="10" t="inlineStr"/>
+      <c r="C70" s="11" t="inlineStr">
         <is>
           <t>24/Dec/2025</t>
         </is>
       </c>
-      <c r="D70" s="1" t="inlineStr">
+      <c r="D70" s="9" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E70" s="7" t="inlineStr">
+      <c r="E70" s="12" t="inlineStr">
         <is>
           <t>Brac Bank PLC-CD-A/C-2028701210002</t>
         </is>
       </c>
-      <c r="F70" s="1" t="inlineStr"/>
-      <c r="G70" s="1" t="inlineStr"/>
-      <c r="H70" s="25" t="inlineStr">
+      <c r="F70" s="9" t="inlineStr"/>
+      <c r="G70" s="9" t="inlineStr"/>
+      <c r="H70" s="13" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I70" s="1" t="inlineStr">
+      <c r="I70" s="9" t="inlineStr">
         <is>
           <t>67</t>
         </is>
       </c>
-      <c r="J70" s="1" t="inlineStr"/>
-      <c r="K70" s="8" t="inlineStr">
+      <c r="J70" s="9" t="inlineStr"/>
+      <c r="K70" s="14" t="inlineStr">
         <is>
           <t>45000000</t>
         </is>
       </c>
-      <c r="L70" s="1" t="inlineStr"/>
+      <c r="L70" s="9" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr"/>
-      <c r="B71" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Borrower's narration does not contain lender's short code</t>
-        </is>
-      </c>
-      <c r="C71" s="1" t="inlineStr"/>
-      <c r="D71" s="1" t="inlineStr"/>
-      <c r="E71" s="26" t="inlineStr">
+      <c r="A71" s="9" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B71" s="10" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 45000000.00
+Borrower Amount: 45000000.00</t>
+        </is>
+      </c>
+      <c r="C71" s="9" t="inlineStr"/>
+      <c r="D71" s="9" t="inlineStr"/>
+      <c r="E71" s="15" t="inlineStr">
         <is>
           <t>Interunit Funs Transfer as Interunit Loan A/C-Steel Unit, MTB# 1105</t>
         </is>
       </c>
-      <c r="F71" s="1" t="inlineStr"/>
-      <c r="G71" s="1" t="inlineStr"/>
-      <c r="H71" s="1" t="inlineStr"/>
-      <c r="I71" s="1" t="inlineStr"/>
-      <c r="J71" s="1" t="inlineStr"/>
-      <c r="K71" s="1" t="inlineStr"/>
-      <c r="L71" s="1" t="inlineStr"/>
+      <c r="F71" s="9" t="inlineStr"/>
+      <c r="G71" s="9" t="inlineStr"/>
+      <c r="H71" s="9" t="inlineStr"/>
+      <c r="I71" s="9" t="inlineStr"/>
+      <c r="J71" s="9" t="inlineStr"/>
+      <c r="K71" s="9" t="inlineStr"/>
+      <c r="L71" s="9" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr"/>
-      <c r="B72" s="2" t="inlineStr"/>
-      <c r="C72" s="1" t="inlineStr"/>
-      <c r="D72" s="1" t="inlineStr">
+      <c r="A72" s="9" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B72" s="10" t="inlineStr"/>
+      <c r="C72" s="9" t="inlineStr"/>
+      <c r="D72" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E72" s="27" t="inlineStr">
+      <c r="E72" s="16" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F72" s="1" t="inlineStr"/>
-      <c r="G72" s="1" t="inlineStr"/>
-      <c r="H72" s="1" t="inlineStr"/>
-      <c r="I72" s="1" t="inlineStr"/>
-      <c r="J72" s="1" t="inlineStr"/>
-      <c r="K72" s="1" t="inlineStr"/>
-      <c r="L72" s="1" t="inlineStr"/>
+      <c r="F72" s="9" t="inlineStr"/>
+      <c r="G72" s="9" t="inlineStr"/>
+      <c r="H72" s="9" t="inlineStr"/>
+      <c r="I72" s="9" t="inlineStr"/>
+      <c r="J72" s="9" t="inlineStr"/>
+      <c r="K72" s="9" t="inlineStr"/>
+      <c r="L72" s="9" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr"/>
-      <c r="B73" s="2" t="inlineStr"/>
-      <c r="C73" s="6" t="inlineStr">
+      <c r="A73" s="17" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B73" s="18" t="inlineStr"/>
+      <c r="C73" s="19" t="inlineStr">
         <is>
           <t>28/Dec/2025</t>
         </is>
       </c>
-      <c r="D73" s="1" t="inlineStr">
+      <c r="D73" s="17" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E73" s="7" t="inlineStr">
+      <c r="E73" s="20" t="inlineStr">
         <is>
           <t>Brac Bank PLC-CD-A/C-2028701210002</t>
         </is>
       </c>
-      <c r="F73" s="1" t="inlineStr"/>
-      <c r="G73" s="1" t="inlineStr"/>
-      <c r="H73" s="25" t="inlineStr">
+      <c r="F73" s="17" t="inlineStr"/>
+      <c r="G73" s="17" t="inlineStr"/>
+      <c r="H73" s="21" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I73" s="1" t="inlineStr">
+      <c r="I73" s="17" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="J73" s="1" t="inlineStr"/>
-      <c r="K73" s="8" t="inlineStr">
+      <c r="J73" s="17" t="inlineStr"/>
+      <c r="K73" s="22" t="inlineStr">
         <is>
           <t>100000</t>
         </is>
       </c>
-      <c r="L73" s="1" t="inlineStr"/>
+      <c r="L73" s="17" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr"/>
-      <c r="B74" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Borrower's narration does not contain lender's short code</t>
-        </is>
-      </c>
-      <c r="C74" s="1" t="inlineStr"/>
-      <c r="D74" s="1" t="inlineStr"/>
-      <c r="E74" s="26" t="inlineStr">
+      <c r="A74" s="17" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B74" s="18" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 100000.00
+Borrower Amount: 100000.00</t>
+        </is>
+      </c>
+      <c r="C74" s="17" t="inlineStr"/>
+      <c r="D74" s="17" t="inlineStr"/>
+      <c r="E74" s="23" t="inlineStr">
         <is>
           <t>Interunit Funs Transfer as Interunit Loan A/C-Steel Unit, MTB# 1105</t>
         </is>
       </c>
-      <c r="F74" s="1" t="inlineStr"/>
-      <c r="G74" s="1" t="inlineStr"/>
-      <c r="H74" s="1" t="inlineStr"/>
-      <c r="I74" s="1" t="inlineStr"/>
-      <c r="J74" s="1" t="inlineStr"/>
-      <c r="K74" s="1" t="inlineStr"/>
-      <c r="L74" s="1" t="inlineStr"/>
+      <c r="F74" s="17" t="inlineStr"/>
+      <c r="G74" s="17" t="inlineStr"/>
+      <c r="H74" s="17" t="inlineStr"/>
+      <c r="I74" s="17" t="inlineStr"/>
+      <c r="J74" s="17" t="inlineStr"/>
+      <c r="K74" s="17" t="inlineStr"/>
+      <c r="L74" s="17" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr"/>
-      <c r="B75" s="2" t="inlineStr"/>
-      <c r="C75" s="1" t="inlineStr"/>
-      <c r="D75" s="1" t="inlineStr">
+      <c r="A75" s="17" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B75" s="18" t="inlineStr"/>
+      <c r="C75" s="17" t="inlineStr"/>
+      <c r="D75" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E75" s="27" t="inlineStr">
+      <c r="E75" s="24" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F75" s="1" t="inlineStr"/>
-      <c r="G75" s="1" t="inlineStr"/>
-      <c r="H75" s="1" t="inlineStr"/>
-      <c r="I75" s="1" t="inlineStr"/>
-      <c r="J75" s="1" t="inlineStr"/>
-      <c r="K75" s="1" t="inlineStr"/>
-      <c r="L75" s="1" t="inlineStr"/>
+      <c r="F75" s="17" t="inlineStr"/>
+      <c r="G75" s="17" t="inlineStr"/>
+      <c r="H75" s="17" t="inlineStr"/>
+      <c r="I75" s="17" t="inlineStr"/>
+      <c r="J75" s="17" t="inlineStr"/>
+      <c r="K75" s="17" t="inlineStr"/>
+      <c r="L75" s="17" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="9" t="inlineStr">
@@ -3210,7 +3249,7 @@
     <row r="82">
       <c r="A82" s="9" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="B82" s="10" t="inlineStr"/>
@@ -3256,7 +3295,7 @@
     <row r="83">
       <c r="A83" s="9" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="B83" s="10" t="inlineStr">
@@ -3288,7 +3327,7 @@
     <row r="84">
       <c r="A84" s="9" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="B84" s="10" t="inlineStr"/>
@@ -3330,7 +3369,7 @@
       <c r="H85" s="1" t="inlineStr"/>
       <c r="I85" s="1" t="inlineStr"/>
       <c r="J85" s="1" t="inlineStr"/>
-      <c r="K85" s="28" t="inlineStr">
+      <c r="K85" s="25" t="inlineStr">
         <is>
           <t>413172115.16</t>
         </is>
@@ -3378,7 +3417,7 @@
       <c r="H87" s="1" t="inlineStr"/>
       <c r="I87" s="1" t="inlineStr"/>
       <c r="J87" s="1" t="inlineStr"/>
-      <c r="K87" s="28" t="inlineStr">
+      <c r="K87" s="25" t="inlineStr">
         <is>
           <t>413172115.16</t>
         </is>

</xml_diff>